<commit_message>
Progress made on run_model function, but some values doverging to infinity
</commit_message>
<xml_diff>
--- a/CIVE 625/Lab1.xlsx
+++ b/CIVE 625/Lab1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adunw\OneDrive\Documents\GitHub\EcoHydro\CIVE 625\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617419FE-8F9B-4396-94D5-D375754517D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678B7E07-C577-43C0-93F0-A193342562FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,42 +380,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>u</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>surface</t>
     </r>
   </si>
   <si>
@@ -1512,17 +1476,77 @@
     <t xml:space="preserve"> Precip</t>
   </si>
   <si>
-    <t>lambda</t>
-  </si>
-  <si>
     <t>delta</t>
-  </si>
-  <si>
-    <t>psyc</t>
   </si>
   <si>
     <r>
       <t>lambda*E</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>total</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Zm' </t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>LW_down</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Tk</t>
+  </si>
+  <si>
+    <t>SW_in</t>
+  </si>
+  <si>
+    <t>psy_const</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <r>
+      <t>lambdaE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>lambdaE</t>
     </r>
     <r>
       <rPr>
@@ -1574,7 +1598,7 @@
   </si>
   <si>
     <r>
-      <t>lambda*E</t>
+      <t>T</t>
     </r>
     <r>
       <rPr>
@@ -1587,12 +1611,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>T</t>
+      <t>s</t>
     </r>
   </si>
   <si>
     <r>
-      <t>lambda*E</t>
+      <t>LW_</t>
     </r>
     <r>
       <rPr>
@@ -1605,32 +1629,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>total</t>
+      <t>up</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Zm' </t>
-  </si>
-  <si>
-    <t>um</t>
-  </si>
-  <si>
-    <t>Ta</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>LW_down</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>Tk</t>
-  </si>
-  <si>
-    <t>SW_in</t>
   </si>
 </sst>
 </file>
@@ -23856,6 +23856,60 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>37</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>43</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5145" name="Object 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s5145"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82CEE33E-D655-4F7D-9745-09F04B2D99A8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -25334,7 +25388,7 @@
   <dimension ref="A1:AJ204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25362,7 +25416,7 @@
     <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.7109375" customWidth="1"/>
     <col min="24" max="24" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" customWidth="1"/>
     <col min="26" max="26" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -25377,7 +25431,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="19"/>
@@ -25386,11 +25440,11 @@
       <c r="F1" s="21"/>
       <c r="G1" s="22"/>
       <c r="H1" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I1" s="24"/>
       <c r="J1" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K1" s="26"/>
       <c r="L1" s="27"/>
@@ -25421,13 +25475,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G2" s="30" t="s">
         <v>21</v>
@@ -25436,58 +25490,58 @@
         <v>7</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" s="34" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L2" s="35" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N2" s="36" t="s">
         <v>20</v>
       </c>
       <c r="O2" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="R2" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="35" t="s">
+      <c r="T2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="35" t="s">
+      <c r="U2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="V2" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="35" t="s">
+      <c r="W2" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="35" t="s">
+      <c r="Y2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="37" t="s">
         <v>53</v>
-      </c>
-      <c r="Y2" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" s="37" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25501,7 +25555,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>19</v>
@@ -25531,16 +25585,16 @@
         <v>4</v>
       </c>
       <c r="N3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="Q3" s="42" t="s">
         <v>58</v>
-      </c>
-      <c r="P3" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="42" t="s">
-        <v>60</v>
       </c>
       <c r="R3" s="42" t="s">
         <v>11</v>
@@ -25555,13 +25609,13 @@
         <v>4</v>
       </c>
       <c r="V3" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="X3" s="42" t="s">
         <v>61</v>
-      </c>
-      <c r="W3" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="X3" s="42" t="s">
-        <v>63</v>
       </c>
       <c r="Y3" s="41" t="s">
         <v>4</v>
@@ -25656,17 +25710,17 @@
     </row>
     <row r="5" spans="1:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F5" s="4">
         <v>22</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="68" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I5" s="68" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5"/>
@@ -25682,7 +25736,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F6" s="1">
         <v>22</v>
@@ -25721,7 +25775,7 @@
       <c r="L7" s="92"/>
       <c r="M7" s="93"/>
       <c r="N7" s="94" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O7" s="92"/>
       <c r="P7" s="92"/>
@@ -25730,7 +25784,7 @@
       <c r="S7" s="92"/>
       <c r="T7" s="92"/>
       <c r="U7" s="161" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="V7" s="106"/>
       <c r="W7" s="111"/>
@@ -25738,14 +25792,14 @@
       <c r="Y7" s="112"/>
       <c r="Z7" s="111"/>
       <c r="AA7" s="112" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AB7" s="111"/>
       <c r="AC7" s="114"/>
       <c r="AD7" s="113"/>
       <c r="AE7" s="111"/>
       <c r="AF7" s="112" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AG7" s="115"/>
       <c r="AH7" s="111"/>
@@ -25754,7 +25808,7 @@
     </row>
     <row r="8" spans="1:36" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -25764,28 +25818,28 @@
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
       <c r="I8" s="97" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="173"/>
       <c r="K8" s="86"/>
       <c r="L8" s="86"/>
       <c r="M8" s="91"/>
       <c r="N8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R8" s="85"/>
       <c r="S8" s="86"/>
       <c r="T8" s="155" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U8" s="162"/>
       <c r="V8" s="107"/>
@@ -25806,87 +25860,87 @@
     </row>
     <row r="9" spans="1:36" ht="18.75" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C9" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="F9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="73" t="s">
+      <c r="G9" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="16" t="s">
+      <c r="H9" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="H9" s="74" t="s">
-        <v>121</v>
-      </c>
       <c r="I9" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="175" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="175" t="s">
-        <v>72</v>
-      </c>
-      <c r="K9" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="84" t="s">
-        <v>73</v>
-      </c>
       <c r="M9" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="N9" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="P9" s="86" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="N9" s="86" t="s">
-        <v>77</v>
-      </c>
-      <c r="O9" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="P9" s="86" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q9" s="86" t="s">
-        <v>80</v>
-      </c>
-      <c r="R9" s="86" t="s">
-        <v>85</v>
-      </c>
       <c r="S9" s="85" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T9" s="155" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U9" s="181" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V9" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="W9" s="159" t="s">
         <v>92</v>
       </c>
-      <c r="W9" s="159" t="s">
+      <c r="X9" s="119" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y9" s="120" t="s">
         <v>94</v>
-      </c>
-      <c r="X9" s="119" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y9" s="120" t="s">
-        <v>96</v>
       </c>
       <c r="Z9" s="100"/>
       <c r="AA9" s="100"/>
       <c r="AB9" s="100"/>
       <c r="AC9" s="101"/>
       <c r="AD9" s="102" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AE9" s="100"/>
       <c r="AF9" s="102" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AG9" s="102" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AH9" s="117"/>
       <c r="AI9" s="117"/>
@@ -25948,7 +26002,7 @@
         <v>19</v>
       </c>
       <c r="S10" s="88" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T10" s="157" t="s">
         <v>8</v>
@@ -26004,28 +26058,28 @@
     </row>
     <row r="11" spans="1:36" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="69" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" s="71" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E11" s="73" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F11" s="73" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H11" s="74" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I11" s="96" t="s">
         <v>27</v>
@@ -26040,7 +26094,7 @@
         <v>14</v>
       </c>
       <c r="M11" s="90" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="N11" s="90" t="s">
         <v>29</v>
@@ -26052,10 +26106,10 @@
         <v>31</v>
       </c>
       <c r="Q11" s="90" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R11" s="90" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S11" s="90" t="s">
         <v>32</v>
@@ -26064,52 +26118,52 @@
         <v>33</v>
       </c>
       <c r="U11" s="163" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="V11" s="108" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W11" s="102" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="X11" s="102" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Y11" s="102" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="Z11" s="104" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AA11" s="104" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AB11" s="75" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AC11" s="105" t="s">
         <v>22</v>
       </c>
       <c r="AD11" s="104" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AE11" s="104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AF11" s="104" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="AG11" s="104" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AH11" s="123" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AI11" s="123" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="AJ11" s="121" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:36" s="192" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -36389,6 +36443,31 @@
         <oleObject progId="Equation.DSMT4" shapeId="5144" r:id="rId23"/>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.DSMT4" shapeId="5145" r:id="rId25">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId12">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>37</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>43</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.DSMT4" shapeId="5145" r:id="rId25"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -36414,25 +36493,25 @@
     <row r="38" spans="19:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="19:25" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="S39" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="T39" s="131" t="s">
+        <v>101</v>
+      </c>
+      <c r="U39" s="132" t="s">
+        <v>102</v>
+      </c>
+      <c r="V39" s="131" t="s">
+        <v>35</v>
+      </c>
+      <c r="W39" s="132" t="s">
+        <v>103</v>
+      </c>
+      <c r="X39" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="T39" s="131" t="s">
-        <v>103</v>
-      </c>
-      <c r="U39" s="132" t="s">
+      <c r="Y39" s="134" t="s">
         <v>104</v>
-      </c>
-      <c r="V39" s="131" t="s">
-        <v>37</v>
-      </c>
-      <c r="W39" s="132" t="s">
-        <v>105</v>
-      </c>
-      <c r="X39" s="133" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y39" s="134" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="40" spans="19:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -36684,7 +36763,7 @@
   <dimension ref="A1:AT204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36735,7 +36814,7 @@
   <sheetData>
     <row r="1" spans="1:46" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="19"/>
@@ -36744,11 +36823,11 @@
       <c r="F1" s="21"/>
       <c r="G1" s="22"/>
       <c r="H1" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I1" s="24"/>
       <c r="J1" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K1" s="26"/>
       <c r="L1" s="27"/>
@@ -36778,13 +36857,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G2" s="53" t="s">
         <v>21</v>
@@ -36793,58 +36872,58 @@
         <v>7</v>
       </c>
       <c r="I2" s="55" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" s="56" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L2" s="57" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N2" s="58" t="s">
         <v>20</v>
       </c>
       <c r="O2" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="57" t="s">
+      <c r="R2" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="S2" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="57" t="s">
+      <c r="T2" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="U2" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="57" t="s">
+      <c r="V2" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="57" t="s">
+      <c r="W2" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="57" t="s">
+      <c r="X2" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="59" t="s">
+      <c r="Y2" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="X2" s="57" t="s">
+      <c r="Z2" s="60" t="s">
         <v>53</v>
-      </c>
-      <c r="Y2" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" s="60" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:46" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -36858,7 +36937,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>19</v>
@@ -36888,16 +36967,16 @@
         <v>4</v>
       </c>
       <c r="N3" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="66" t="s">
+      <c r="Q3" s="63" t="s">
         <v>58</v>
-      </c>
-      <c r="P3" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="63" t="s">
-        <v>60</v>
       </c>
       <c r="R3" s="63" t="s">
         <v>11</v>
@@ -36912,13 +36991,13 @@
         <v>4</v>
       </c>
       <c r="V3" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="X3" s="63" t="s">
         <v>61</v>
-      </c>
-      <c r="W3" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="X3" s="63" t="s">
-        <v>63</v>
       </c>
       <c r="Y3" s="65" t="s">
         <v>4</v>
@@ -37013,17 +37092,17 @@
     </row>
     <row r="5" spans="1:46" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="68" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I5" s="68" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5"/>
@@ -37034,7 +37113,7 @@
     </row>
     <row r="6" spans="1:46" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -37046,7 +37125,7 @@
     </row>
     <row r="8" spans="1:46" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -37056,28 +37135,28 @@
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
       <c r="I8" s="97" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="173"/>
       <c r="K8" s="86"/>
       <c r="L8" s="86"/>
       <c r="M8" s="91"/>
       <c r="N8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R8" s="85"/>
       <c r="S8" s="86"/>
       <c r="T8" s="155" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U8" s="162"/>
       <c r="V8" s="107"/>
@@ -37105,87 +37184,87 @@
     </row>
     <row r="9" spans="1:46" ht="18.75" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C9" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="F9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="73" t="s">
+      <c r="G9" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="16" t="s">
+      <c r="H9" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="H9" s="74" t="s">
-        <v>121</v>
-      </c>
       <c r="I9" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="175" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="175" t="s">
-        <v>72</v>
-      </c>
-      <c r="K9" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="84" t="s">
-        <v>73</v>
-      </c>
       <c r="M9" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="N9" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="P9" s="86" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="N9" s="86" t="s">
-        <v>77</v>
-      </c>
-      <c r="O9" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="P9" s="86" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q9" s="86" t="s">
-        <v>80</v>
-      </c>
-      <c r="R9" s="86" t="s">
-        <v>85</v>
-      </c>
       <c r="S9" s="85" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T9" s="155" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="U9" s="181" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V9" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="W9" s="159" t="s">
         <v>92</v>
       </c>
-      <c r="W9" s="159" t="s">
+      <c r="X9" s="119" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y9" s="120" t="s">
         <v>94</v>
-      </c>
-      <c r="X9" s="119" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y9" s="120" t="s">
-        <v>96</v>
       </c>
       <c r="Z9" s="100"/>
       <c r="AA9" s="100"/>
       <c r="AB9" s="100"/>
       <c r="AC9" s="101"/>
       <c r="AD9" s="102" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AE9" s="100"/>
       <c r="AF9" s="102" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AG9" s="102" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AH9" s="117"/>
       <c r="AI9" s="117"/>
@@ -37254,7 +37333,7 @@
         <v>19</v>
       </c>
       <c r="S10" s="88" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T10" s="157" t="s">
         <v>8</v>
@@ -37317,28 +37396,28 @@
     </row>
     <row r="11" spans="1:46" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="69" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" s="71" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E11" s="73" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F11" s="73" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H11" s="74" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I11" s="96" t="s">
         <v>27</v>
@@ -37353,7 +37432,7 @@
         <v>14</v>
       </c>
       <c r="M11" s="90" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="N11" s="90" t="s">
         <v>29</v>
@@ -37365,10 +37444,10 @@
         <v>31</v>
       </c>
       <c r="Q11" s="90" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R11" s="90" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S11" s="90" t="s">
         <v>32</v>
@@ -37377,52 +37456,52 @@
         <v>33</v>
       </c>
       <c r="U11" s="163" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="V11" s="108" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="W11" s="102" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="X11" s="102" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Y11" s="102" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="Z11" s="104" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AA11" s="104" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AB11" s="75" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AC11" s="105" t="s">
         <v>22</v>
       </c>
       <c r="AD11" s="104" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AE11" s="104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AF11" s="104" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="AG11" s="104" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="AH11" s="123" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AI11" s="123" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="AJ11" s="121" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AN11"/>
       <c r="AO11"/>
@@ -47924,25 +48003,25 @@
     <row r="38" spans="19:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="19:25" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="S39" s="130" t="s">
+        <v>34</v>
+      </c>
+      <c r="T39" s="131" t="s">
+        <v>101</v>
+      </c>
+      <c r="U39" s="132" t="s">
+        <v>102</v>
+      </c>
+      <c r="V39" s="131" t="s">
+        <v>35</v>
+      </c>
+      <c r="W39" s="132" t="s">
+        <v>103</v>
+      </c>
+      <c r="X39" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="T39" s="131" t="s">
-        <v>103</v>
-      </c>
-      <c r="U39" s="132" t="s">
+      <c r="Y39" s="134" t="s">
         <v>104</v>
-      </c>
-      <c r="V39" s="131" t="s">
-        <v>37</v>
-      </c>
-      <c r="W39" s="132" t="s">
-        <v>105</v>
-      </c>
-      <c r="X39" s="133" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y39" s="134" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="40" spans="19:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>